<commit_message>
Thermal Neutrom Porosity is renamed to Neutron Porosity
</commit_message>
<xml_diff>
--- a/components/petrophysics/data/src/FluidMineralConstants.xlsx
+++ b/components/petrophysics/data/src/FluidMineralConstants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20372"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dIcEmAN\Docker\petrotool\components\importexport\rules\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dIcEmAN\Docker\petrotool\components\petrophysics\data\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5D0A3B-00D5-4633-8FC5-85FEA12551A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC16D4B7-EB7E-4EC3-A7BC-8F4706286C70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7380" yWindow="1965" windowWidth="21600" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t>Bulk Density</t>
   </si>
   <si>
-    <t>Thermal Neutron Porosity</t>
-  </si>
-  <si>
     <t>Gamma Ray</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>Units</t>
+  </si>
+  <si>
+    <t>Neutron Porosity</t>
   </si>
 </sst>
 </file>
@@ -414,9 +414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -429,36 +427,36 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -480,7 +478,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="b">
         <v>1</v>
@@ -497,7 +495,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
update: families, familtproperties and mineralconstrains
Co-authored-by: Aleksey Lubinets <lubinetsab@gmail.com>
</commit_message>
<xml_diff>
--- a/components/petrophysics/data/src/FluidMineralConstants.xlsx
+++ b/components/petrophysics/data/src/FluidMineralConstants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20374"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dIcEmAN\Docker\petrotool\components\petrophysics\data\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\senat\programming\petrotool\components\petrophysics\data\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08146ABF-3831-4A18-85A8-589422C347C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE6E5D1-31D6-47CD-8D35-AA1CC7357379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,12 +23,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="96">
   <si>
     <t>Shale</t>
   </si>
@@ -304,6 +313,18 @@
   </si>
   <si>
     <t>Log Family</t>
+  </si>
+  <si>
+    <t>unitless</t>
+  </si>
+  <si>
+    <t>Spontaneous Potential</t>
+  </si>
+  <si>
+    <t>mV</t>
+  </si>
+  <si>
+    <t>Neutron Far</t>
   </si>
 </sst>
 </file>
@@ -675,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,14 +711,15 @@
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" customWidth="1"/>
-    <col min="11" max="11" width="17.7109375" customWidth="1"/>
-    <col min="12" max="12" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="16.7109375" style="6" customWidth="1"/>
+    <col min="10" max="10" width="21.140625" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" customWidth="1"/>
+    <col min="14" max="14" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -720,25 +742,31 @@
         <v>84</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -760,26 +788,32 @@
       <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="J2" t="s">
         <v>77</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>74</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>3</v>
-      </c>
-      <c r="K2" t="s">
-        <v>75</v>
-      </c>
-      <c r="L2" t="s">
-        <v>76</v>
       </c>
       <c r="M2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>76</v>
+      </c>
+      <c r="O2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -801,26 +835,26 @@
       <c r="G3" s="6">
         <v>0.3</v>
       </c>
-      <c r="H3" s="6">
+      <c r="J3" s="6">
         <v>2.33</v>
       </c>
-      <c r="I3" s="6">
+      <c r="K3" s="6">
         <v>4.32</v>
       </c>
-      <c r="J3" s="6">
+      <c r="L3" s="6">
         <v>2.77</v>
       </c>
-      <c r="K3" s="6">
+      <c r="M3" s="6">
         <v>11.8094</v>
       </c>
-      <c r="L3" s="6">
+      <c r="N3" s="6">
         <v>6.45</v>
       </c>
-      <c r="M3" s="6">
+      <c r="O3" s="6">
         <v>4.6085000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -842,26 +876,26 @@
       <c r="G4" s="6">
         <v>0.37</v>
       </c>
-      <c r="H4" s="6">
+      <c r="J4" s="6">
         <v>2.0499999999999998</v>
       </c>
-      <c r="I4" s="6">
+      <c r="K4" s="6">
         <v>0.1</v>
       </c>
-      <c r="J4" s="6">
+      <c r="L4" s="6">
         <v>2.41</v>
       </c>
-      <c r="K4" s="6">
+      <c r="M4" s="6">
         <v>18.859100000000002</v>
       </c>
-      <c r="L4" s="6">
+      <c r="N4" s="6">
         <v>5.0999999999999996</v>
       </c>
-      <c r="M4" s="6">
+      <c r="O4" s="6">
         <v>3.1269</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
@@ -883,26 +917,26 @@
       <c r="G5" s="6">
         <v>0.218</v>
       </c>
-      <c r="H5" s="6">
+      <c r="J5" s="6">
         <v>2.89</v>
       </c>
-      <c r="I5" s="6">
+      <c r="K5" s="6">
         <v>0.48</v>
       </c>
-      <c r="J5" s="6">
+      <c r="L5" s="6">
         <v>2.78</v>
       </c>
-      <c r="K5" s="6">
+      <c r="M5" s="6">
         <v>20.626999999999999</v>
       </c>
-      <c r="L5" s="6">
+      <c r="N5" s="6">
         <v>4.4000000000000004</v>
       </c>
-      <c r="M5" s="6">
+      <c r="O5" s="6">
         <v>5.6327999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -924,26 +958,26 @@
       <c r="G6" s="6">
         <v>0.218</v>
       </c>
-      <c r="H6" s="6">
+      <c r="J6" s="6">
         <v>1.26</v>
       </c>
-      <c r="I6" s="6">
+      <c r="K6" s="6">
         <v>0.48</v>
       </c>
-      <c r="J6" s="6">
+      <c r="L6" s="6">
         <v>2.12</v>
       </c>
-      <c r="K6" s="6">
+      <c r="M6" s="6">
         <v>20.626999999999999</v>
       </c>
-      <c r="L6" s="6">
+      <c r="N6" s="6">
         <v>2.63</v>
       </c>
-      <c r="M6" s="6">
+      <c r="O6" s="6">
         <v>5.6327999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -965,26 +999,26 @@
       <c r="G7" s="6">
         <v>0.52</v>
       </c>
-      <c r="H7" s="6">
+      <c r="J7" s="6">
         <v>8.06</v>
       </c>
-      <c r="I7" s="6">
+      <c r="K7" s="6">
         <v>0.37</v>
       </c>
-      <c r="J7" s="6">
+      <c r="L7" s="6">
         <v>2.76</v>
       </c>
-      <c r="K7" s="6">
+      <c r="M7" s="6">
         <v>10.99</v>
       </c>
-      <c r="L7" s="6">
+      <c r="N7" s="6">
         <v>21.7</v>
       </c>
-      <c r="M7" s="6">
+      <c r="O7" s="6">
         <v>3.4704999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
@@ -1006,26 +1040,26 @@
       <c r="G8" s="6">
         <v>0.52</v>
       </c>
-      <c r="H8" s="6">
+      <c r="J8" s="6">
         <v>6.73</v>
       </c>
-      <c r="I8" s="6">
+      <c r="K8" s="6">
         <v>5.9</v>
       </c>
-      <c r="J8" s="6">
+      <c r="L8" s="6">
         <v>2.85</v>
       </c>
-      <c r="K8" s="6">
+      <c r="M8" s="6">
         <v>10.99</v>
       </c>
-      <c r="L8" s="6">
+      <c r="N8" s="6">
         <v>19.100000000000001</v>
       </c>
-      <c r="M8" s="6">
+      <c r="O8" s="6">
         <v>4.6085000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
@@ -1048,25 +1082,31 @@
         <v>0.4</v>
       </c>
       <c r="H9" s="6">
+        <v>1</v>
+      </c>
+      <c r="I9" s="6">
+        <v>150</v>
+      </c>
+      <c r="J9" s="6">
         <v>4</v>
       </c>
-      <c r="I9" s="6">
+      <c r="K9" s="6">
         <v>5</v>
       </c>
-      <c r="J9" s="6">
+      <c r="L9" s="6">
         <v>2.4500000000000002</v>
       </c>
-      <c r="K9" s="6">
+      <c r="M9" s="6">
         <v>15</v>
       </c>
-      <c r="L9" s="6">
+      <c r="N9" s="6">
         <v>10</v>
       </c>
-      <c r="M9" s="6">
+      <c r="O9" s="6">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>1</v>
       </c>
@@ -1089,25 +1129,31 @@
         <v>-0.03</v>
       </c>
       <c r="H10" s="6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I10" s="6">
+        <v>20</v>
+      </c>
+      <c r="J10" s="6">
         <v>1.9</v>
       </c>
-      <c r="I10" s="6">
-        <v>0</v>
-      </c>
-      <c r="J10" s="6">
+      <c r="K10" s="6">
+        <v>0</v>
+      </c>
+      <c r="L10" s="6">
         <v>2.65</v>
       </c>
-      <c r="K10" s="6">
-        <v>0</v>
-      </c>
-      <c r="L10" s="6">
+      <c r="M10" s="6">
+        <v>0</v>
+      </c>
+      <c r="N10" s="6">
         <v>5</v>
       </c>
-      <c r="M10" s="6">
+      <c r="O10" s="6">
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1129,26 +1175,26 @@
       <c r="G11" s="6">
         <v>0.02</v>
       </c>
-      <c r="H11" s="6">
+      <c r="J11" s="6">
         <v>3.38</v>
       </c>
-      <c r="I11" s="6">
+      <c r="K11" s="6">
         <v>10.199999999999999</v>
       </c>
-      <c r="J11" s="6">
+      <c r="L11" s="6">
         <v>2.57</v>
       </c>
-      <c r="K11" s="6">
+      <c r="M11" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="L11" s="6">
+      <c r="N11" s="6">
         <v>8.6999999999999993</v>
       </c>
-      <c r="M11" s="6">
+      <c r="O11" s="6">
         <v>0.4</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
@@ -1170,26 +1216,26 @@
       <c r="G12" s="6">
         <v>-5.0000000000000001E-3</v>
       </c>
-      <c r="H12" s="6">
+      <c r="J12" s="6">
         <v>2.13</v>
       </c>
-      <c r="I12" s="6">
+      <c r="K12" s="6">
         <v>0.5</v>
       </c>
-      <c r="J12" s="6">
+      <c r="L12" s="6">
         <v>2.61</v>
       </c>
-      <c r="K12" s="6">
-        <v>0</v>
-      </c>
-      <c r="L12" s="6">
+      <c r="M12" s="6">
+        <v>0</v>
+      </c>
+      <c r="N12" s="6">
         <v>5.6</v>
       </c>
-      <c r="M12" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O12" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>17</v>
       </c>
@@ -1211,26 +1257,26 @@
       <c r="G13" s="6">
         <v>-8.0000000000000002E-3</v>
       </c>
-      <c r="H13" s="6">
+      <c r="J13" s="6">
         <v>3.05</v>
       </c>
-      <c r="I13" s="6">
-        <v>0</v>
-      </c>
-      <c r="J13" s="6">
+      <c r="K13" s="6">
+        <v>0</v>
+      </c>
+      <c r="L13" s="6">
         <v>2.76</v>
       </c>
-      <c r="K13" s="6">
-        <v>0</v>
-      </c>
-      <c r="L13" s="6">
+      <c r="M13" s="6">
+        <v>0</v>
+      </c>
+      <c r="N13" s="6">
         <v>8.4</v>
       </c>
-      <c r="M13" s="6">
+      <c r="O13" s="6">
         <v>0.1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
@@ -1252,26 +1298,26 @@
       <c r="G14" s="6">
         <v>0.2</v>
       </c>
-      <c r="H14" s="6">
+      <c r="J14" s="6">
         <v>7.04</v>
       </c>
-      <c r="I14" s="6">
+      <c r="K14" s="6">
         <v>7.2</v>
       </c>
-      <c r="J14" s="6">
+      <c r="L14" s="6">
         <v>3.09</v>
       </c>
-      <c r="K14" s="6">
+      <c r="M14" s="6">
         <v>1.5</v>
       </c>
-      <c r="L14" s="6">
+      <c r="N14" s="6">
         <v>21.6</v>
       </c>
-      <c r="M14" s="6">
+      <c r="O14" s="6">
         <v>0.7</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1293,26 +1339,26 @@
       <c r="G15" s="6">
         <v>0.2</v>
       </c>
-      <c r="H15" s="6">
+      <c r="J15" s="6">
         <v>4.04</v>
       </c>
-      <c r="I15" s="6">
+      <c r="K15" s="6">
         <v>7.8</v>
       </c>
-      <c r="J15" s="6">
+      <c r="L15" s="6">
         <v>2.86</v>
       </c>
-      <c r="K15" s="6">
-        <v>0</v>
-      </c>
-      <c r="L15" s="6">
+      <c r="M15" s="6">
+        <v>0</v>
+      </c>
+      <c r="N15" s="6">
         <v>11.5</v>
       </c>
-      <c r="M15" s="6">
+      <c r="O15" s="6">
         <v>0.7</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>2</v>
       </c>
@@ -1335,25 +1381,31 @@
         <v>0</v>
       </c>
       <c r="H16" s="6">
+        <v>6</v>
+      </c>
+      <c r="I16" s="6">
+        <v>0</v>
+      </c>
+      <c r="J16" s="6">
         <v>5.22</v>
       </c>
-      <c r="I16" s="6">
-        <v>0</v>
-      </c>
-      <c r="J16" s="6">
+      <c r="K16" s="6">
+        <v>0</v>
+      </c>
+      <c r="L16" s="6">
         <v>2.71</v>
       </c>
-      <c r="K16" s="6">
-        <v>0</v>
-      </c>
-      <c r="L16" s="6">
+      <c r="M16" s="6">
+        <v>0</v>
+      </c>
+      <c r="N16" s="6">
         <v>14.1</v>
       </c>
-      <c r="M16" s="6">
+      <c r="O16" s="6">
         <v>1.4</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
@@ -1375,26 +1427,26 @@
       <c r="G17" s="6">
         <v>0.03</v>
       </c>
-      <c r="H17" s="6">
+      <c r="J17" s="6">
         <v>3.36</v>
       </c>
-      <c r="I17" s="6">
-        <v>0</v>
-      </c>
-      <c r="J17" s="6">
+      <c r="K17" s="6">
+        <v>0</v>
+      </c>
+      <c r="L17" s="6">
         <v>2.87</v>
       </c>
-      <c r="K17" s="6">
+      <c r="M17" s="6">
         <v>0.1</v>
       </c>
-      <c r="L17" s="6">
+      <c r="N17" s="6">
         <v>9.1</v>
       </c>
-      <c r="M17" s="6">
+      <c r="O17" s="6">
         <v>0.9</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>21</v>
       </c>
@@ -1416,26 +1468,26 @@
       <c r="G18" s="6">
         <v>0.06</v>
       </c>
-      <c r="H18" s="6">
+      <c r="J18" s="6">
         <v>9.32</v>
       </c>
-      <c r="I18" s="6">
+      <c r="K18" s="6">
         <v>7</v>
       </c>
-      <c r="J18" s="6">
+      <c r="L18" s="6">
         <v>2.96</v>
       </c>
-      <c r="K18" s="6">
-        <v>0</v>
-      </c>
-      <c r="L18" s="6">
+      <c r="M18" s="6">
+        <v>0</v>
+      </c>
+      <c r="N18" s="6">
         <v>27.6</v>
       </c>
-      <c r="M18" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O18" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>22</v>
       </c>
@@ -1457,26 +1509,26 @@
       <c r="G19" s="6">
         <v>-0.03</v>
       </c>
-      <c r="H19" s="6">
+      <c r="J19" s="6">
         <v>4.7</v>
       </c>
-      <c r="I19" s="6">
-        <v>0</v>
-      </c>
-      <c r="J19" s="6">
+      <c r="K19" s="6">
+        <v>0</v>
+      </c>
+      <c r="L19" s="6">
         <v>2.04</v>
       </c>
-      <c r="K19" s="6">
-        <v>0</v>
-      </c>
-      <c r="L19" s="6">
+      <c r="M19" s="6">
+        <v>0</v>
+      </c>
+      <c r="N19" s="6">
         <v>9.6999999999999993</v>
       </c>
-      <c r="M19" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O19" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>23</v>
       </c>
@@ -1498,26 +1550,26 @@
       <c r="G20" s="6">
         <v>-0.03</v>
       </c>
-      <c r="H20" s="6">
+      <c r="J20" s="6">
         <v>5.0999999999999996</v>
       </c>
-      <c r="I20" s="6">
-        <v>0</v>
-      </c>
-      <c r="J20" s="6">
+      <c r="K20" s="6">
+        <v>0</v>
+      </c>
+      <c r="L20" s="6">
         <v>2.98</v>
       </c>
-      <c r="K20" s="6">
-        <v>0</v>
-      </c>
-      <c r="L20" s="6">
+      <c r="M20" s="6">
+        <v>0</v>
+      </c>
+      <c r="N20" s="6">
         <v>14.95</v>
       </c>
-      <c r="M20" s="6">
+      <c r="O20" s="6">
         <v>0.4</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>24</v>
       </c>
@@ -1539,26 +1591,26 @@
       <c r="G21" s="6">
         <v>0.6</v>
       </c>
-      <c r="H21" s="6">
+      <c r="J21" s="6">
         <v>4</v>
       </c>
-      <c r="I21" s="6">
-        <v>0</v>
-      </c>
-      <c r="J21" s="6">
+      <c r="K21" s="6">
+        <v>0</v>
+      </c>
+      <c r="L21" s="6">
         <v>2.35</v>
       </c>
-      <c r="K21" s="6">
-        <v>0</v>
-      </c>
-      <c r="L21" s="6">
+      <c r="M21" s="6">
+        <v>0</v>
+      </c>
+      <c r="N21" s="6">
         <v>9.4</v>
       </c>
-      <c r="M21" s="6">
+      <c r="O21" s="6">
         <v>0.3</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>25</v>
       </c>
@@ -1580,26 +1632,26 @@
       <c r="G22" s="6">
         <v>-0.03</v>
       </c>
-      <c r="H22" s="6">
+      <c r="J22" s="6">
         <v>1.7</v>
       </c>
-      <c r="I22" s="6">
-        <v>0</v>
-      </c>
-      <c r="J22" s="6">
+      <c r="K22" s="6">
+        <v>0</v>
+      </c>
+      <c r="L22" s="6">
         <v>2.15</v>
       </c>
-      <c r="K22" s="6">
-        <v>0</v>
-      </c>
-      <c r="L22" s="6">
+      <c r="M22" s="6">
+        <v>0</v>
+      </c>
+      <c r="N22" s="6">
         <v>3.5</v>
       </c>
-      <c r="M22" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O22" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>26</v>
       </c>
@@ -1621,26 +1673,26 @@
       <c r="G23" s="6">
         <v>-0.03</v>
       </c>
-      <c r="H23" s="6">
+      <c r="J23" s="6">
         <v>70</v>
       </c>
-      <c r="I23" s="6">
-        <v>0</v>
-      </c>
-      <c r="J23" s="6">
+      <c r="K23" s="6">
+        <v>0</v>
+      </c>
+      <c r="L23" s="6">
         <v>4.5</v>
-      </c>
-      <c r="K23" s="6">
-        <v>1000</v>
-      </c>
-      <c r="L23" s="6">
-        <v>310</v>
       </c>
       <c r="M23" s="6">
         <v>1000</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23" s="6">
+        <v>310</v>
+      </c>
+      <c r="O23" s="6">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>27</v>
       </c>
@@ -1662,26 +1714,26 @@
       <c r="G24" s="6">
         <v>-0.03</v>
       </c>
-      <c r="H24" s="6">
+      <c r="J24" s="6">
         <v>17</v>
       </c>
-      <c r="I24" s="6">
-        <v>0</v>
-      </c>
-      <c r="J24" s="6">
+      <c r="K24" s="6">
+        <v>0</v>
+      </c>
+      <c r="L24" s="6">
         <v>4.99</v>
       </c>
-      <c r="K24" s="6">
-        <v>0</v>
-      </c>
-      <c r="L24" s="6">
+      <c r="M24" s="6">
+        <v>0</v>
+      </c>
+      <c r="N24" s="6">
         <v>82.06</v>
       </c>
-      <c r="M24" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O24" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>28</v>
       </c>
@@ -1703,26 +1755,26 @@
       <c r="G25" s="6">
         <v>0.01</v>
       </c>
-      <c r="H25" s="6">
+      <c r="J25" s="6">
         <v>266</v>
       </c>
-      <c r="I25" s="6">
+      <c r="K25" s="6">
         <v>0.1</v>
       </c>
-      <c r="J25" s="6">
+      <c r="L25" s="6">
         <v>4.08</v>
-      </c>
-      <c r="K25" s="6">
-        <v>1E-3</v>
-      </c>
-      <c r="L25" s="6">
-        <v>1065</v>
       </c>
       <c r="M25" s="6">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N25" s="6">
+        <v>1065</v>
+      </c>
+      <c r="O25" s="6">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>29</v>
       </c>
@@ -1744,26 +1796,26 @@
       <c r="G26" s="6">
         <v>0.1</v>
       </c>
-      <c r="H26" s="6">
+      <c r="J26" s="6">
         <v>18.63</v>
       </c>
-      <c r="I26" s="6">
-        <v>0</v>
-      </c>
-      <c r="J26" s="6">
+      <c r="K26" s="6">
+        <v>0</v>
+      </c>
+      <c r="L26" s="6">
         <v>3.93</v>
       </c>
-      <c r="K26" s="6">
+      <c r="M26" s="6">
         <v>0.4</v>
       </c>
-      <c r="L26" s="6">
+      <c r="N26" s="6">
         <v>71.599999999999994</v>
       </c>
-      <c r="M26" s="6">
+      <c r="O26" s="6">
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>30</v>
       </c>
@@ -1785,26 +1837,26 @@
       <c r="G27" s="6">
         <v>0.65</v>
       </c>
-      <c r="H27" s="6">
+      <c r="J27" s="6">
         <v>0.2</v>
       </c>
-      <c r="I27" s="6">
-        <v>0</v>
-      </c>
-      <c r="J27" s="6">
+      <c r="K27" s="6">
+        <v>0</v>
+      </c>
+      <c r="L27" s="6">
         <v>1.4</v>
       </c>
-      <c r="K27" s="6">
-        <v>0</v>
-      </c>
-      <c r="L27" s="6">
+      <c r="M27" s="6">
+        <v>0</v>
+      </c>
+      <c r="N27" s="6">
         <v>0.3</v>
       </c>
-      <c r="M27" s="6">
+      <c r="O27" s="6">
         <v>1000</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>31</v>
       </c>
@@ -1826,26 +1878,26 @@
       <c r="G28" s="6">
         <v>0.6</v>
       </c>
-      <c r="H28" s="6">
+      <c r="J28" s="6">
         <v>0.2</v>
       </c>
-      <c r="I28" s="6">
-        <v>0</v>
-      </c>
-      <c r="J28" s="6">
+      <c r="K28" s="6">
+        <v>0</v>
+      </c>
+      <c r="L28" s="6">
         <v>1.5</v>
       </c>
-      <c r="K28" s="6">
-        <v>0</v>
-      </c>
-      <c r="L28" s="6">
+      <c r="M28" s="6">
+        <v>0</v>
+      </c>
+      <c r="N28" s="6">
         <v>0.2</v>
       </c>
-      <c r="M28" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O28" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>32</v>
       </c>
@@ -1867,26 +1919,26 @@
       <c r="G29" s="6">
         <v>0</v>
       </c>
-      <c r="H29" s="6">
+      <c r="J29" s="6">
         <v>6</v>
       </c>
-      <c r="I29" s="6">
+      <c r="K29" s="6">
         <v>7</v>
       </c>
-      <c r="J29" s="6">
+      <c r="L29" s="6">
         <v>2.68</v>
       </c>
-      <c r="K29" s="6">
+      <c r="M29" s="6">
         <v>8</v>
       </c>
-      <c r="L29" s="6">
+      <c r="N29" s="6">
         <v>16</v>
       </c>
-      <c r="M29" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O29" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>33</v>
       </c>
@@ -1908,26 +1960,26 @@
       <c r="G30" s="6">
         <v>1</v>
       </c>
-      <c r="H30" s="6">
+      <c r="J30" s="6">
         <v>0.36</v>
       </c>
-      <c r="I30" s="6">
-        <v>0</v>
-      </c>
-      <c r="J30" s="6">
+      <c r="K30" s="6">
+        <v>0</v>
+      </c>
+      <c r="L30" s="6">
         <v>1</v>
       </c>
-      <c r="K30" s="6">
-        <v>0</v>
-      </c>
-      <c r="L30" s="6">
+      <c r="M30" s="6">
+        <v>0</v>
+      </c>
+      <c r="N30" s="6">
         <v>0.4</v>
       </c>
-      <c r="M30" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O30" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>34</v>
       </c>
@@ -1950,25 +2002,31 @@
         <v>1</v>
       </c>
       <c r="H31" s="6">
+        <v>5</v>
+      </c>
+      <c r="I31" s="6">
+        <v>0</v>
+      </c>
+      <c r="J31" s="6">
         <v>0.36</v>
       </c>
-      <c r="I31" s="6">
-        <v>0</v>
-      </c>
-      <c r="J31" s="6">
+      <c r="K31" s="6">
+        <v>0</v>
+      </c>
+      <c r="L31" s="6">
         <v>1.05</v>
       </c>
-      <c r="K31" s="6">
-        <v>0</v>
-      </c>
-      <c r="L31" s="6">
+      <c r="M31" s="6">
+        <v>0</v>
+      </c>
+      <c r="N31" s="6">
         <v>0.4</v>
       </c>
-      <c r="M31" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O31" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>35</v>
       </c>
@@ -1990,26 +2048,26 @@
       <c r="G32" s="6">
         <v>0.95</v>
       </c>
-      <c r="H32" s="6">
+      <c r="J32" s="6">
         <v>0.12</v>
       </c>
-      <c r="I32" s="6">
-        <v>0</v>
-      </c>
-      <c r="J32" s="6">
+      <c r="K32" s="6">
+        <v>0</v>
+      </c>
+      <c r="L32" s="6">
         <v>0.7</v>
       </c>
-      <c r="K32" s="6">
-        <v>0</v>
-      </c>
-      <c r="L32" s="6">
+      <c r="M32" s="6">
+        <v>0</v>
+      </c>
+      <c r="N32" s="6">
         <v>0.11</v>
       </c>
-      <c r="M32" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O32" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>36</v>
       </c>
@@ -2031,12 +2089,6 @@
       <c r="G33" s="6">
         <v>0.2</v>
       </c>
-      <c r="H33" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="I33" s="6">
-        <v>0</v>
-      </c>
       <c r="J33" s="6">
         <v>0.1</v>
       </c>
@@ -2044,13 +2096,19 @@
         <v>0</v>
       </c>
       <c r="L33" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="M33" s="6">
+        <v>0</v>
+      </c>
+      <c r="N33" s="6">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M33" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O33" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>37</v>
       </c>
@@ -2073,25 +2131,31 @@
         <v>1</v>
       </c>
       <c r="H34" s="6">
+        <v>5</v>
+      </c>
+      <c r="I34" s="6">
+        <v>0</v>
+      </c>
+      <c r="J34" s="6">
         <v>0.36</v>
       </c>
-      <c r="I34" s="6">
-        <v>0</v>
-      </c>
-      <c r="J34" s="6">
+      <c r="K34" s="6">
+        <v>0</v>
+      </c>
+      <c r="L34" s="6">
         <v>1.05</v>
       </c>
-      <c r="K34" s="6">
-        <v>0</v>
-      </c>
-      <c r="L34" s="6">
+      <c r="M34" s="6">
+        <v>0</v>
+      </c>
+      <c r="N34" s="6">
         <v>0.4</v>
       </c>
-      <c r="M34" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O34" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>38</v>
       </c>
@@ -2113,26 +2177,26 @@
       <c r="G35" s="6">
         <v>0.95</v>
       </c>
-      <c r="H35" s="6">
+      <c r="J35" s="6">
         <v>0.12</v>
       </c>
-      <c r="I35" s="6">
-        <v>0</v>
-      </c>
-      <c r="J35" s="6">
+      <c r="K35" s="6">
+        <v>0</v>
+      </c>
+      <c r="L35" s="6">
         <v>0.7</v>
       </c>
-      <c r="K35" s="6">
-        <v>0</v>
-      </c>
-      <c r="L35" s="6">
+      <c r="M35" s="6">
+        <v>0</v>
+      </c>
+      <c r="N35" s="6">
         <v>0.11</v>
       </c>
-      <c r="M35" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O35" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>39</v>
       </c>
@@ -2154,12 +2218,6 @@
       <c r="G36" s="6">
         <v>0.2</v>
       </c>
-      <c r="H36" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="I36" s="6">
-        <v>0</v>
-      </c>
       <c r="J36" s="6">
         <v>0.1</v>
       </c>
@@ -2167,9 +2225,15 @@
         <v>0</v>
       </c>
       <c r="L36" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="M36" s="6">
+        <v>0</v>
+      </c>
+      <c r="N36" s="6">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M36" s="6">
+      <c r="O36" s="6">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
VM with log weights
</commit_message>
<xml_diff>
--- a/components/petrophysics/data/src/FluidMineralConstants.xlsx
+++ b/components/petrophysics/data/src/FluidMineralConstants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20377"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\senat\programming\petrotool\components\petrophysics\data\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dIcEmAN\Docker\petrotool\components\petrophysics\data\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE6E5D1-31D6-47CD-8D35-AA1CC7357379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79875D3-B2EA-4F3A-8D93-5CC36234B9A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,28 +16,19 @@
     <sheet name="Constants" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Constants!$A$2:$F$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Constants!$A$2:$F$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="97">
   <si>
     <t>Shale</t>
   </si>
@@ -63,9 +54,6 @@
     <t>Component</t>
   </si>
   <si>
-    <t>Units</t>
-  </si>
-  <si>
     <t>Illite</t>
   </si>
   <si>
@@ -325,6 +313,12 @@
   </si>
   <si>
     <t>Neutron Far</t>
+  </si>
+  <si>
+    <t>_units</t>
+  </si>
+  <si>
+    <t>_weight</t>
   </si>
 </sst>
 </file>
@@ -696,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O36"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,63 +718,63 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -789,162 +783,164 @@
         <v>4</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L2" t="s">
         <v>3</v>
       </c>
       <c r="M2" t="s">
+        <v>74</v>
+      </c>
+      <c r="N2" t="s">
         <v>75</v>
       </c>
-      <c r="N2" t="s">
-        <v>76</v>
-      </c>
       <c r="O2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="3">
-        <v>295.27559055118081</v>
-      </c>
-      <c r="E3" s="3">
-        <v>426.50918635170558</v>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.8</v>
       </c>
       <c r="F3" s="6">
-        <v>150</v>
+        <v>0.7</v>
       </c>
       <c r="G3" s="6">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="I3" s="6">
         <v>0.3</v>
       </c>
       <c r="J3" s="6">
-        <v>2.33</v>
+        <v>1</v>
       </c>
       <c r="K3" s="6">
-        <v>4.32</v>
+        <v>1</v>
       </c>
       <c r="L3" s="6">
-        <v>2.77</v>
+        <v>1</v>
       </c>
       <c r="M3" s="6">
-        <v>11.8094</v>
+        <v>1</v>
       </c>
       <c r="N3" s="6">
-        <v>6.45</v>
+        <v>1</v>
       </c>
       <c r="O3" s="6">
-        <v>4.6085000000000003</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D4" s="3">
-        <v>262.46719160104959</v>
+        <v>295.27559055118081</v>
       </c>
       <c r="E4" s="3">
-        <v>360.8923884514432</v>
+        <v>426.50918635170558</v>
       </c>
       <c r="F4" s="6">
-        <v>98</v>
+        <v>150</v>
       </c>
       <c r="G4" s="6">
-        <v>0.37</v>
+        <v>0.3</v>
       </c>
       <c r="J4" s="6">
-        <v>2.0499999999999998</v>
+        <v>2.33</v>
       </c>
       <c r="K4" s="6">
-        <v>0.1</v>
+        <v>4.32</v>
       </c>
       <c r="L4" s="6">
-        <v>2.41</v>
+        <v>2.77</v>
       </c>
       <c r="M4" s="6">
-        <v>18.859100000000002</v>
+        <v>11.8094</v>
       </c>
       <c r="N4" s="6">
-        <v>5.0999999999999996</v>
+        <v>6.45</v>
       </c>
       <c r="O4" s="6">
-        <v>3.1269</v>
+        <v>4.6085000000000003</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D5" s="3">
-        <v>393.70078740157442</v>
+        <v>262.46719160104959</v>
       </c>
       <c r="E5" s="3">
-        <v>524.93438320209918</v>
+        <v>360.8923884514432</v>
       </c>
       <c r="F5" s="6">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G5" s="6">
-        <v>0.218</v>
+        <v>0.37</v>
       </c>
       <c r="J5" s="6">
-        <v>2.89</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="K5" s="6">
-        <v>0.48</v>
+        <v>0.1</v>
       </c>
       <c r="L5" s="6">
-        <v>2.78</v>
+        <v>2.41</v>
       </c>
       <c r="M5" s="6">
-        <v>20.626999999999999</v>
+        <v>18.859100000000002</v>
       </c>
       <c r="N5" s="6">
-        <v>4.4000000000000004</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="O5" s="6">
-        <v>5.6327999999999996</v>
+        <v>3.1269</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D6" s="3">
         <v>393.70078740157442</v>
@@ -953,25 +949,25 @@
         <v>524.93438320209918</v>
       </c>
       <c r="F6" s="6">
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="G6" s="6">
         <v>0.218</v>
       </c>
       <c r="J6" s="6">
-        <v>1.26</v>
+        <v>2.89</v>
       </c>
       <c r="K6" s="6">
         <v>0.48</v>
       </c>
       <c r="L6" s="6">
-        <v>2.12</v>
+        <v>2.78</v>
       </c>
       <c r="M6" s="6">
         <v>20.626999999999999</v>
       </c>
       <c r="N6" s="6">
-        <v>2.63</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="O6" s="6">
         <v>5.6327999999999996</v>
@@ -979,380 +975,380 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D7" s="3">
-        <v>262.46719160104959</v>
+        <v>393.70078740157442</v>
       </c>
       <c r="E7" s="3">
-        <v>328.08398950131198</v>
+        <v>524.93438320209918</v>
       </c>
       <c r="F7" s="6">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="G7" s="6">
-        <v>0.52</v>
+        <v>0.218</v>
       </c>
       <c r="J7" s="6">
-        <v>8.06</v>
+        <v>1.26</v>
       </c>
       <c r="K7" s="6">
-        <v>0.37</v>
+        <v>0.48</v>
       </c>
       <c r="L7" s="6">
-        <v>2.76</v>
+        <v>2.12</v>
       </c>
       <c r="M7" s="6">
-        <v>10.99</v>
+        <v>20.626999999999999</v>
       </c>
       <c r="N7" s="6">
-        <v>21.7</v>
+        <v>2.63</v>
       </c>
       <c r="O7" s="6">
-        <v>3.4704999999999999</v>
+        <v>5.6327999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D8" s="3">
-        <v>295.27559055118081</v>
+        <v>262.46719160104959</v>
       </c>
       <c r="E8" s="3">
-        <v>426.50918635170558</v>
+        <v>328.08398950131198</v>
       </c>
       <c r="F8" s="6">
-        <v>150</v>
+        <v>74</v>
       </c>
       <c r="G8" s="6">
         <v>0.52</v>
       </c>
       <c r="J8" s="6">
-        <v>6.73</v>
+        <v>8.06</v>
       </c>
       <c r="K8" s="6">
-        <v>5.9</v>
+        <v>0.37</v>
       </c>
       <c r="L8" s="6">
-        <v>2.85</v>
+        <v>2.76</v>
       </c>
       <c r="M8" s="6">
         <v>10.99</v>
       </c>
       <c r="N8" s="6">
-        <v>19.100000000000001</v>
+        <v>21.7</v>
       </c>
       <c r="O8" s="6">
-        <v>4.6085000000000003</v>
+        <v>3.4704999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D9" s="3">
-        <v>328.08398950131198</v>
+        <v>295.27559055118081</v>
       </c>
       <c r="E9" s="3">
-        <v>574.14698162729599</v>
+        <v>426.50918635170558</v>
       </c>
       <c r="F9" s="6">
         <v>150</v>
       </c>
       <c r="G9" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="H9" s="6">
-        <v>1</v>
-      </c>
-      <c r="I9" s="6">
-        <v>150</v>
+        <v>0.52</v>
       </c>
       <c r="J9" s="6">
-        <v>4</v>
+        <v>6.73</v>
       </c>
       <c r="K9" s="6">
-        <v>5</v>
+        <v>5.9</v>
       </c>
       <c r="L9" s="6">
-        <v>2.4500000000000002</v>
+        <v>2.85</v>
       </c>
       <c r="M9" s="6">
-        <v>15</v>
+        <v>10.99</v>
       </c>
       <c r="N9" s="6">
-        <v>10</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="O9" s="6">
-        <v>9</v>
+        <v>4.6085000000000003</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D10" s="3">
-        <v>182.08661417322816</v>
+        <v>328.08398950131198</v>
       </c>
       <c r="E10" s="3">
-        <v>242.78215223097087</v>
+        <v>574.14698162729599</v>
       </c>
       <c r="F10" s="6">
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="G10" s="6">
-        <v>-0.03</v>
+        <v>0.4</v>
       </c>
       <c r="H10" s="6">
-        <v>2.2000000000000002</v>
+        <v>1</v>
       </c>
       <c r="I10" s="6">
-        <v>20</v>
+        <v>150</v>
       </c>
       <c r="J10" s="6">
-        <v>1.9</v>
+        <v>4</v>
       </c>
       <c r="K10" s="6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L10" s="6">
-        <v>2.65</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="M10" s="6">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="N10" s="6">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="O10" s="6">
-        <v>0.1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D11" s="3">
-        <v>196.85039370078721</v>
+        <v>182.08661417322816</v>
       </c>
       <c r="E11" s="3">
-        <v>305.38057742782121</v>
+        <v>242.78215223097087</v>
       </c>
       <c r="F11" s="6">
-        <v>170</v>
+        <v>30</v>
       </c>
       <c r="G11" s="6">
-        <v>0.02</v>
+        <v>-0.03</v>
+      </c>
+      <c r="H11" s="6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I11" s="6">
+        <v>20</v>
       </c>
       <c r="J11" s="6">
-        <v>3.38</v>
+        <v>1.9</v>
       </c>
       <c r="K11" s="6">
-        <v>10.199999999999999</v>
+        <v>0</v>
       </c>
       <c r="L11" s="6">
-        <v>2.57</v>
+        <v>2.65</v>
       </c>
       <c r="M11" s="6">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="N11" s="6">
-        <v>8.6999999999999993</v>
+        <v>5</v>
       </c>
       <c r="O11" s="6">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D12" s="3">
-        <v>160.76115485564287</v>
+        <v>196.85039370078721</v>
       </c>
       <c r="E12" s="3">
-        <v>296.71916010498654</v>
+        <v>305.38057742782121</v>
       </c>
       <c r="F12" s="6">
-        <v>8</v>
+        <v>170</v>
       </c>
       <c r="G12" s="6">
-        <v>-5.0000000000000001E-3</v>
+        <v>0.02</v>
       </c>
       <c r="J12" s="6">
-        <v>2.13</v>
+        <v>3.38</v>
       </c>
       <c r="K12" s="6">
-        <v>0.5</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="L12" s="6">
-        <v>2.61</v>
+        <v>2.57</v>
       </c>
       <c r="M12" s="6">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="N12" s="6">
-        <v>5.6</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="O12" s="6">
-        <v>0</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D13" s="3">
-        <v>180.4461942257216</v>
+        <v>160.76115485564287</v>
       </c>
       <c r="E13" s="3">
-        <v>305.11811023622016</v>
+        <v>296.71916010498654</v>
       </c>
       <c r="F13" s="6">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G13" s="6">
-        <v>-8.0000000000000002E-3</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="J13" s="6">
-        <v>3.05</v>
+        <v>2.13</v>
       </c>
       <c r="K13" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L13" s="6">
-        <v>2.76</v>
+        <v>2.61</v>
       </c>
       <c r="M13" s="6">
         <v>0</v>
       </c>
       <c r="N13" s="6">
-        <v>8.4</v>
+        <v>5.6</v>
       </c>
       <c r="O13" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D14" s="3">
-        <v>196.85039370078721</v>
+        <v>180.4461942257216</v>
       </c>
       <c r="E14" s="3">
-        <v>295.27559055118081</v>
+        <v>305.11811023622016</v>
       </c>
       <c r="F14" s="6">
-        <v>127</v>
+        <v>1</v>
       </c>
       <c r="G14" s="6">
-        <v>0.2</v>
+        <v>-8.0000000000000002E-3</v>
       </c>
       <c r="J14" s="6">
-        <v>7.04</v>
+        <v>3.05</v>
       </c>
       <c r="K14" s="6">
-        <v>7.2</v>
+        <v>0</v>
       </c>
       <c r="L14" s="6">
-        <v>3.09</v>
+        <v>2.76</v>
       </c>
       <c r="M14" s="6">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="N14" s="6">
-        <v>21.6</v>
+        <v>8.4</v>
       </c>
       <c r="O14" s="6">
-        <v>0.7</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D15" s="3">
-        <v>173.88451443569537</v>
+        <v>196.85039370078721</v>
       </c>
       <c r="E15" s="3">
         <v>295.27559055118081</v>
       </c>
       <c r="F15" s="6">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G15" s="6">
         <v>0.2</v>
       </c>
       <c r="J15" s="6">
-        <v>4.04</v>
+        <v>7.04</v>
       </c>
       <c r="K15" s="6">
-        <v>7.8</v>
+        <v>7.2</v>
       </c>
       <c r="L15" s="6">
-        <v>2.86</v>
+        <v>3.09</v>
       </c>
       <c r="M15" s="6">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="N15" s="6">
-        <v>11.5</v>
+        <v>21.6</v>
       </c>
       <c r="O15" s="6">
         <v>0.7</v>
@@ -1360,169 +1356,169 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D16" s="3">
-        <v>155.8398950131232</v>
+        <v>173.88451443569537</v>
       </c>
       <c r="E16" s="3">
-        <v>291.01049868766376</v>
+        <v>295.27559055118081</v>
       </c>
       <c r="F16" s="6">
-        <v>11</v>
+        <v>130</v>
       </c>
       <c r="G16" s="6">
-        <v>0</v>
-      </c>
-      <c r="H16" s="6">
-        <v>6</v>
-      </c>
-      <c r="I16" s="6">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="J16" s="6">
-        <v>5.22</v>
+        <v>4.04</v>
       </c>
       <c r="K16" s="6">
-        <v>0</v>
+        <v>7.8</v>
       </c>
       <c r="L16" s="6">
-        <v>2.71</v>
+        <v>2.86</v>
       </c>
       <c r="M16" s="6">
         <v>0</v>
       </c>
       <c r="N16" s="6">
-        <v>14.1</v>
+        <v>11.5</v>
       </c>
       <c r="O16" s="6">
-        <v>1.4</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D17" s="3">
-        <v>142.7165354330707</v>
+        <v>155.8398950131232</v>
       </c>
       <c r="E17" s="3">
-        <v>255.90551181102336</v>
+        <v>291.01049868766376</v>
       </c>
       <c r="F17" s="6">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G17" s="6">
-        <v>0.03</v>
+        <v>0</v>
+      </c>
+      <c r="H17" s="6">
+        <v>6</v>
+      </c>
+      <c r="I17" s="6">
+        <v>0</v>
       </c>
       <c r="J17" s="6">
-        <v>3.36</v>
+        <v>5.22</v>
       </c>
       <c r="K17" s="6">
         <v>0</v>
       </c>
       <c r="L17" s="6">
-        <v>2.87</v>
+        <v>2.71</v>
       </c>
       <c r="M17" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="N17" s="6">
-        <v>9.1</v>
+        <v>14.1</v>
       </c>
       <c r="O17" s="6">
-        <v>0.9</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B18" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D18" s="3">
-        <v>144.35695538057729</v>
+        <v>142.7165354330707</v>
       </c>
       <c r="E18" s="3">
-        <v>236.22047244094463</v>
+        <v>255.90551181102336</v>
       </c>
       <c r="F18" s="6">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G18" s="6">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="J18" s="6">
-        <v>9.32</v>
+        <v>3.36</v>
       </c>
       <c r="K18" s="6">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="L18" s="6">
-        <v>2.96</v>
+        <v>2.87</v>
       </c>
       <c r="M18" s="6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="N18" s="6">
-        <v>27.6</v>
+        <v>9.1</v>
       </c>
       <c r="O18" s="6">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D19" s="3">
-        <v>219.81627296587902</v>
+        <v>144.35695538057729</v>
       </c>
       <c r="E19" s="3">
-        <v>393.70078740157442</v>
+        <v>236.22047244094463</v>
       </c>
       <c r="F19" s="6">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G19" s="6">
-        <v>-0.03</v>
+        <v>0.06</v>
       </c>
       <c r="J19" s="6">
-        <v>4.7</v>
+        <v>9.32</v>
       </c>
       <c r="K19" s="6">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L19" s="6">
-        <v>2.04</v>
+        <v>2.96</v>
       </c>
       <c r="M19" s="6">
         <v>0</v>
       </c>
       <c r="N19" s="6">
-        <v>9.6999999999999993</v>
+        <v>27.6</v>
       </c>
       <c r="O19" s="6">
         <v>0</v>
@@ -1530,341 +1526,341 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B20" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D20" s="3">
-        <v>164.04199475065599</v>
+        <v>219.81627296587902</v>
       </c>
       <c r="E20" s="3">
-        <v>301.83727034120705</v>
+        <v>393.70078740157442</v>
       </c>
       <c r="F20" s="6">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G20" s="6">
         <v>-0.03</v>
       </c>
       <c r="J20" s="6">
-        <v>5.0999999999999996</v>
+        <v>4.7</v>
       </c>
       <c r="K20" s="6">
         <v>0</v>
       </c>
       <c r="L20" s="6">
-        <v>2.98</v>
+        <v>2.04</v>
       </c>
       <c r="M20" s="6">
         <v>0</v>
       </c>
       <c r="N20" s="6">
-        <v>14.95</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="O20" s="6">
-        <v>0.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B21" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D21" s="3">
-        <v>170.60367454068222</v>
+        <v>164.04199475065599</v>
       </c>
       <c r="E21" s="3">
-        <v>308.39895013123328</v>
+        <v>301.83727034120705</v>
       </c>
       <c r="F21" s="6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G21" s="6">
-        <v>0.6</v>
+        <v>-0.03</v>
       </c>
       <c r="J21" s="6">
-        <v>4</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="K21" s="6">
         <v>0</v>
       </c>
       <c r="L21" s="6">
-        <v>2.35</v>
+        <v>2.98</v>
       </c>
       <c r="M21" s="6">
         <v>0</v>
       </c>
       <c r="N21" s="6">
-        <v>9.4</v>
+        <v>14.95</v>
       </c>
       <c r="O21" s="6">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B22" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D22" s="3">
-        <v>190.28871391076095</v>
+        <v>170.60367454068222</v>
       </c>
       <c r="E22" s="3">
-        <v>328.08398950131198</v>
+        <v>308.39895013123328</v>
       </c>
       <c r="F22" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22" s="6">
-        <v>-0.03</v>
+        <v>0.6</v>
       </c>
       <c r="J22" s="6">
-        <v>1.7</v>
+        <v>4</v>
       </c>
       <c r="K22" s="6">
         <v>0</v>
       </c>
       <c r="L22" s="6">
-        <v>2.15</v>
+        <v>2.35</v>
       </c>
       <c r="M22" s="6">
         <v>0</v>
       </c>
       <c r="N22" s="6">
-        <v>3.5</v>
+        <v>9.4</v>
       </c>
       <c r="O22" s="6">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B23" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D23" s="3">
-        <v>196.85039370078721</v>
+        <v>190.28871391076095</v>
       </c>
       <c r="E23" s="3">
-        <v>249.34383202099713</v>
+        <v>328.08398950131198</v>
       </c>
       <c r="F23" s="6">
-        <v>450</v>
+        <v>1</v>
       </c>
       <c r="G23" s="6">
         <v>-0.03</v>
       </c>
       <c r="J23" s="6">
-        <v>70</v>
+        <v>1.7</v>
       </c>
       <c r="K23" s="6">
         <v>0</v>
       </c>
       <c r="L23" s="6">
-        <v>4.5</v>
+        <v>2.15</v>
       </c>
       <c r="M23" s="6">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="N23" s="6">
-        <v>310</v>
+        <v>3.5</v>
       </c>
       <c r="O23" s="6">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B24" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D24" s="3">
-        <v>127.95275590551168</v>
+        <v>196.85039370078721</v>
       </c>
       <c r="E24" s="3">
-        <v>203.74015748031476</v>
+        <v>249.34383202099713</v>
       </c>
       <c r="F24" s="6">
-        <v>0</v>
+        <v>450</v>
       </c>
       <c r="G24" s="6">
         <v>-0.03</v>
       </c>
       <c r="J24" s="6">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="K24" s="6">
         <v>0</v>
       </c>
       <c r="L24" s="6">
-        <v>4.99</v>
+        <v>4.5</v>
       </c>
       <c r="M24" s="6">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="N24" s="6">
-        <v>82.06</v>
+        <v>310</v>
       </c>
       <c r="O24" s="6">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B25" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D25" s="3">
-        <v>228.67454068241446</v>
+        <v>127.95275590551168</v>
       </c>
       <c r="E25" s="3">
-        <v>435.36745406824099</v>
+        <v>203.74015748031476</v>
       </c>
       <c r="F25" s="6">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="G25" s="6">
-        <v>0.01</v>
+        <v>-0.03</v>
       </c>
       <c r="J25" s="6">
-        <v>266</v>
+        <v>17</v>
       </c>
       <c r="K25" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="L25" s="6">
-        <v>4.08</v>
+        <v>4.99</v>
       </c>
       <c r="M25" s="6">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="N25" s="6">
-        <v>1065</v>
+        <v>82.06</v>
       </c>
       <c r="O25" s="6">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B26" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D26" s="3">
-        <v>144.35695538057729</v>
+        <v>228.67454068241446</v>
       </c>
       <c r="E26" s="3">
-        <v>278.54330708661388</v>
+        <v>435.36745406824099</v>
       </c>
       <c r="F26" s="6">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="G26" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="J26" s="6">
+        <v>266</v>
+      </c>
+      <c r="K26" s="6">
         <v>0.1</v>
       </c>
-      <c r="J26" s="6">
-        <v>18.63</v>
-      </c>
-      <c r="K26" s="6">
-        <v>0</v>
-      </c>
       <c r="L26" s="6">
-        <v>3.93</v>
+        <v>4.08</v>
       </c>
       <c r="M26" s="6">
-        <v>0.4</v>
+        <v>1E-3</v>
       </c>
       <c r="N26" s="6">
-        <v>71.599999999999994</v>
+        <v>1065</v>
       </c>
       <c r="O26" s="6">
-        <v>0.5</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B27" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D27" s="3">
-        <v>393.70078740157442</v>
+        <v>144.35695538057729</v>
       </c>
       <c r="E27" s="3">
-        <v>688.97637795275523</v>
+        <v>278.54330708661388</v>
       </c>
       <c r="F27" s="6">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="G27" s="6">
-        <v>0.65</v>
+        <v>0.1</v>
       </c>
       <c r="J27" s="6">
-        <v>0.2</v>
+        <v>18.63</v>
       </c>
       <c r="K27" s="6">
         <v>0</v>
       </c>
       <c r="L27" s="6">
-        <v>1.4</v>
+        <v>3.93</v>
       </c>
       <c r="M27" s="6">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="N27" s="6">
-        <v>0.3</v>
+        <v>71.599999999999994</v>
       </c>
       <c r="O27" s="6">
-        <v>1000</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B28" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D28" s="3">
         <v>393.70078740157442</v>
@@ -1873,10 +1869,10 @@
         <v>688.97637795275523</v>
       </c>
       <c r="F28" s="6">
-        <v>10</v>
+        <v>4000</v>
       </c>
       <c r="G28" s="6">
-        <v>0.6</v>
+        <v>0.65</v>
       </c>
       <c r="J28" s="6">
         <v>0.2</v>
@@ -1885,54 +1881,54 @@
         <v>0</v>
       </c>
       <c r="L28" s="6">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="M28" s="6">
         <v>0</v>
       </c>
       <c r="N28" s="6">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="O28" s="6">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B29" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D29" s="3">
-        <v>213.25459317585279</v>
+        <v>393.70078740157442</v>
       </c>
       <c r="E29" s="3">
-        <v>377.29658792650878</v>
+        <v>688.97637795275523</v>
       </c>
       <c r="F29" s="6">
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="G29" s="6">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="J29" s="6">
-        <v>6</v>
+        <v>0.2</v>
       </c>
       <c r="K29" s="6">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="L29" s="6">
-        <v>2.68</v>
+        <v>1.5</v>
       </c>
       <c r="M29" s="6">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="N29" s="6">
-        <v>16</v>
+        <v>0.2</v>
       </c>
       <c r="O29" s="6">
         <v>0</v>
@@ -1940,40 +1936,40 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B30" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D30" s="3">
-        <v>620.07874015747961</v>
+        <v>213.25459317585279</v>
       </c>
       <c r="E30" s="3">
-        <v>0</v>
+        <v>377.29658792650878</v>
       </c>
       <c r="F30" s="6">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="G30" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" s="6">
-        <v>0.36</v>
+        <v>6</v>
       </c>
       <c r="K30" s="6">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L30" s="6">
-        <v>1</v>
+        <v>2.68</v>
       </c>
       <c r="M30" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N30" s="6">
-        <v>0.4</v>
+        <v>16</v>
       </c>
       <c r="O30" s="6">
         <v>0</v>
@@ -1981,13 +1977,13 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B31" s="2" t="b">
         <v>1</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D31" s="3">
         <v>620.07874015747961</v>
@@ -2001,12 +1997,6 @@
       <c r="G31" s="6">
         <v>1</v>
       </c>
-      <c r="H31" s="6">
-        <v>5</v>
-      </c>
-      <c r="I31" s="6">
-        <v>0</v>
-      </c>
       <c r="J31" s="6">
         <v>0.36</v>
       </c>
@@ -2014,7 +2004,7 @@
         <v>0</v>
       </c>
       <c r="L31" s="6">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="M31" s="6">
         <v>0</v>
@@ -2028,16 +2018,16 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B32" s="2" t="b">
         <v>1</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D32" s="3">
-        <v>688.97637795275523</v>
+        <v>620.07874015747961</v>
       </c>
       <c r="E32" s="3">
         <v>0</v>
@@ -2046,22 +2036,28 @@
         <v>0</v>
       </c>
       <c r="G32" s="6">
-        <v>0.95</v>
+        <v>1</v>
+      </c>
+      <c r="H32" s="6">
+        <v>5</v>
+      </c>
+      <c r="I32" s="6">
+        <v>0</v>
       </c>
       <c r="J32" s="6">
-        <v>0.12</v>
+        <v>0.36</v>
       </c>
       <c r="K32" s="6">
         <v>0</v>
       </c>
       <c r="L32" s="6">
-        <v>0.7</v>
+        <v>1.05</v>
       </c>
       <c r="M32" s="6">
         <v>0</v>
       </c>
       <c r="N32" s="6">
-        <v>0.11</v>
+        <v>0.4</v>
       </c>
       <c r="O32" s="6">
         <v>0</v>
@@ -2069,40 +2065,40 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B33" s="2" t="b">
         <v>1</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D33" s="3">
-        <v>869.4225721784768</v>
+        <v>688.97637795275523</v>
       </c>
       <c r="E33" s="3">
         <v>0</v>
       </c>
       <c r="F33" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33" s="6">
-        <v>0.2</v>
+        <v>0.95</v>
       </c>
       <c r="J33" s="6">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="K33" s="6">
         <v>0</v>
       </c>
       <c r="L33" s="6">
-        <v>0.1</v>
+        <v>0.7</v>
       </c>
       <c r="M33" s="6">
         <v>0</v>
       </c>
       <c r="N33" s="6">
-        <v>1.4999999999999999E-2</v>
+        <v>0.11</v>
       </c>
       <c r="O33" s="6">
         <v>0</v>
@@ -2110,46 +2106,40 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B34" s="2" t="b">
         <v>1</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D34" s="3">
-        <v>620.07874015747961</v>
+        <v>869.4225721784768</v>
       </c>
       <c r="E34" s="3">
         <v>0</v>
       </c>
       <c r="F34" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34" s="6">
-        <v>1</v>
-      </c>
-      <c r="H34" s="6">
-        <v>5</v>
-      </c>
-      <c r="I34" s="6">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="J34" s="6">
-        <v>0.36</v>
+        <v>0.1</v>
       </c>
       <c r="K34" s="6">
         <v>0</v>
       </c>
       <c r="L34" s="6">
-        <v>1.05</v>
+        <v>0.1</v>
       </c>
       <c r="M34" s="6">
         <v>0</v>
       </c>
       <c r="N34" s="6">
-        <v>0.4</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="O34" s="6">
         <v>0</v>
@@ -2157,16 +2147,16 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B35" s="2" t="b">
         <v>1</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D35" s="3">
-        <v>688.97637795275523</v>
+        <v>620.07874015747961</v>
       </c>
       <c r="E35" s="3">
         <v>0</v>
@@ -2175,22 +2165,28 @@
         <v>0</v>
       </c>
       <c r="G35" s="6">
-        <v>0.95</v>
+        <v>1</v>
+      </c>
+      <c r="H35" s="6">
+        <v>5</v>
+      </c>
+      <c r="I35" s="6">
+        <v>0</v>
       </c>
       <c r="J35" s="6">
-        <v>0.12</v>
+        <v>0.36</v>
       </c>
       <c r="K35" s="6">
         <v>0</v>
       </c>
       <c r="L35" s="6">
-        <v>0.7</v>
+        <v>1.05</v>
       </c>
       <c r="M35" s="6">
         <v>0</v>
       </c>
       <c r="N35" s="6">
-        <v>0.11</v>
+        <v>0.4</v>
       </c>
       <c r="O35" s="6">
         <v>0</v>
@@ -2198,42 +2194,83 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B36" s="2" t="b">
         <v>1</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D36" s="3">
+        <v>688.97637795275523</v>
+      </c>
+      <c r="E36" s="3">
+        <v>0</v>
+      </c>
+      <c r="F36" s="6">
+        <v>0</v>
+      </c>
+      <c r="G36" s="6">
+        <v>0.95</v>
+      </c>
+      <c r="J36" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="K36" s="6">
+        <v>0</v>
+      </c>
+      <c r="L36" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="M36" s="6">
+        <v>0</v>
+      </c>
+      <c r="N36" s="6">
+        <v>0.11</v>
+      </c>
+      <c r="O36" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" s="3">
         <v>869.4225721784768</v>
       </c>
-      <c r="E36" s="3">
-        <v>0</v>
-      </c>
-      <c r="F36" s="6">
-        <v>1</v>
-      </c>
-      <c r="G36" s="6">
+      <c r="E37" s="3">
+        <v>0</v>
+      </c>
+      <c r="F37" s="6">
+        <v>1</v>
+      </c>
+      <c r="G37" s="6">
         <v>0.2</v>
       </c>
-      <c r="J36" s="6">
+      <c r="J37" s="6">
         <v>0.1</v>
       </c>
-      <c r="K36" s="6">
-        <v>0</v>
-      </c>
-      <c r="L36" s="6">
+      <c r="K37" s="6">
+        <v>0</v>
+      </c>
+      <c r="L37" s="6">
         <v>0.1</v>
       </c>
-      <c r="M36" s="6">
-        <v>0</v>
-      </c>
-      <c r="N36" s="6">
+      <c r="M37" s="6">
+        <v>0</v>
+      </c>
+      <c r="N37" s="6">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="O36" s="6">
+      <c r="O37" s="6">
         <v>0</v>
       </c>
     </row>

</xml_diff>